<commit_message>
reading workbook, styles, shared strings and sheets
</commit_message>
<xml_diff>
--- a/ExcelReader.Demo/SampleFiles/MultipleSheets.xlsx
+++ b/ExcelReader.Demo/SampleFiles/MultipleSheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1Name" sheetId="1" r:id="rId1"/>
@@ -171,12 +171,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -200,8 +209,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,14 +494,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -542,12 +552,13 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -626,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>